<commit_message>
fix test 7, add ignore list to filter the pay elements we need
</commit_message>
<xml_diff>
--- a/tests/data_case_07_unmapped_payrun_elements/Payrun.xlsx
+++ b/tests/data_case_07_unmapped_payrun_elements/Payrun.xlsx
@@ -835,7 +835,7 @@
     <t>notes</t>
   </si>
   <si>
-    <t>new element</t>
+    <t>test element</t>
   </si>
 </sst>
 </file>
@@ -882,7 +882,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -907,11 +907,13 @@
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Нормален" xfId="0" builtinId="0"/>
@@ -1206,10 +1208,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BC39"/>
+  <dimension ref="A1:BD39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AL11" sqref="AL11"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AM2" sqref="AM2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1241,32 +1243,32 @@
     <col min="32" max="32" width="9.28515625" customWidth="1"/>
     <col min="33" max="33" width="30" customWidth="1"/>
     <col min="34" max="34" width="23.42578125" customWidth="1"/>
-    <col min="35" max="35" width="12.85546875" customWidth="1"/>
-    <col min="36" max="36" width="24.7109375" customWidth="1"/>
-    <col min="37" max="37" width="7" customWidth="1"/>
-    <col min="38" max="38" width="17.42578125" customWidth="1"/>
-    <col min="39" max="39" width="25.85546875" customWidth="1"/>
-    <col min="40" max="40" width="20" customWidth="1"/>
-    <col min="41" max="41" width="11.7109375" customWidth="1"/>
-    <col min="42" max="42" width="24.7109375" customWidth="1"/>
-    <col min="43" max="43" width="5.85546875" customWidth="1"/>
-    <col min="44" max="44" width="25.85546875" customWidth="1"/>
-    <col min="45" max="45" width="23.42578125" customWidth="1"/>
-    <col min="46" max="46" width="15.28515625" customWidth="1"/>
-    <col min="47" max="47" width="12.85546875" customWidth="1"/>
-    <col min="48" max="48" width="9.28515625" customWidth="1"/>
-    <col min="49" max="49" width="30" customWidth="1"/>
-    <col min="50" max="50" width="25.85546875" customWidth="1"/>
-    <col min="51" max="51" width="9.28515625" customWidth="1"/>
-    <col min="52" max="52" width="25.85546875" customWidth="1"/>
-    <col min="53" max="53" width="12.85546875" customWidth="1"/>
-    <col min="54" max="54" width="23.42578125" customWidth="1"/>
-    <col min="55" max="55" width="30" customWidth="1"/>
-    <col min="56" max="1017" width="8.7109375" customWidth="1"/>
-    <col min="1018" max="1026" width="9.140625" customWidth="1"/>
+    <col min="35" max="36" width="12.85546875" customWidth="1"/>
+    <col min="37" max="37" width="24.7109375" customWidth="1"/>
+    <col min="38" max="38" width="7" customWidth="1"/>
+    <col min="39" max="39" width="17.42578125" customWidth="1"/>
+    <col min="40" max="40" width="25.85546875" customWidth="1"/>
+    <col min="41" max="41" width="20" customWidth="1"/>
+    <col min="42" max="42" width="11.7109375" customWidth="1"/>
+    <col min="43" max="43" width="24.7109375" customWidth="1"/>
+    <col min="44" max="44" width="5.85546875" customWidth="1"/>
+    <col min="45" max="45" width="25.85546875" customWidth="1"/>
+    <col min="46" max="46" width="23.42578125" customWidth="1"/>
+    <col min="47" max="47" width="15.28515625" customWidth="1"/>
+    <col min="48" max="48" width="12.85546875" customWidth="1"/>
+    <col min="49" max="49" width="9.28515625" customWidth="1"/>
+    <col min="50" max="50" width="30" customWidth="1"/>
+    <col min="51" max="51" width="25.85546875" customWidth="1"/>
+    <col min="52" max="52" width="9.28515625" customWidth="1"/>
+    <col min="53" max="53" width="25.85546875" customWidth="1"/>
+    <col min="54" max="54" width="12.85546875" customWidth="1"/>
+    <col min="55" max="55" width="23.42578125" customWidth="1"/>
+    <col min="56" max="56" width="30" customWidth="1"/>
+    <col min="57" max="1018" width="8.7109375" customWidth="1"/>
+    <col min="1019" max="1027" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55">
+    <row r="1" spans="1:56">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -1330,7 +1332,7 @@
       <c r="U1" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="13" t="s">
+      <c r="V1" s="15" t="s">
         <v>21</v>
       </c>
       <c r="W1" s="14" t="s">
@@ -1342,62 +1344,63 @@
       <c r="Y1" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="12" t="s">
+      <c r="Z1" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="12"/>
-      <c r="AB1" s="12"/>
-      <c r="AC1" s="12"/>
-      <c r="AD1" s="12"/>
-      <c r="AE1" s="12"/>
-      <c r="AF1" s="12"/>
-      <c r="AG1" s="12"/>
-      <c r="AH1" s="12"/>
-      <c r="AI1" s="12"/>
-      <c r="AJ1" s="12"/>
-      <c r="AK1" s="12"/>
-      <c r="AL1" s="1"/>
-      <c r="AM1" s="2" t="s">
+      <c r="AA1" s="16"/>
+      <c r="AB1" s="16"/>
+      <c r="AC1" s="16"/>
+      <c r="AD1" s="16"/>
+      <c r="AE1" s="16"/>
+      <c r="AF1" s="16"/>
+      <c r="AG1" s="16"/>
+      <c r="AH1" s="16"/>
+      <c r="AI1" s="16"/>
+      <c r="AJ1" s="16"/>
+      <c r="AK1" s="16"/>
+      <c r="AL1" s="16"/>
+      <c r="AM1" s="1"/>
+      <c r="AN1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AO1" s="13" t="s">
+      <c r="AP1" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="AP1" s="13" t="s">
+      <c r="AQ1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="AQ1" s="12" t="s">
+      <c r="AR1" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="AR1" s="12"/>
-      <c r="AS1" s="12"/>
-      <c r="AT1" s="12"/>
-      <c r="AU1" s="13" t="s">
+      <c r="AS1" s="16"/>
+      <c r="AT1" s="16"/>
+      <c r="AU1" s="16"/>
+      <c r="AV1" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="AV1" s="12" t="s">
+      <c r="AW1" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="AW1" s="12"/>
-      <c r="AX1" s="12"/>
-      <c r="AY1" s="13" t="s">
+      <c r="AX1" s="16"/>
+      <c r="AY1" s="16"/>
+      <c r="AZ1" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="AZ1" s="12" t="s">
+      <c r="BA1" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="BA1" s="12"/>
-      <c r="BB1" s="13" t="s">
+      <c r="BB1" s="16"/>
+      <c r="BC1" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="BC1" s="14" t="s">
+      <c r="BD1" s="13" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:55">
+    <row r="2" spans="1:56">
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
@@ -1453,14 +1456,14 @@
       <c r="AI2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="AJ2" s="4" t="s">
+      <c r="AJ2" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="AK2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="AK2" s="4" t="s">
+      <c r="AL2" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="AL2" s="11" t="s">
-        <v>271</v>
       </c>
       <c r="AM2" s="3" t="s">
         <v>49</v>
@@ -1468,8 +1471,8 @@
       <c r="AN2" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="AO2" s="13"/>
-      <c r="AP2" s="13"/>
+      <c r="AO2" s="12"/>
+      <c r="AP2" s="12"/>
       <c r="AQ2" s="3" t="s">
         <v>51</v>
       </c>
@@ -1482,7 +1485,7 @@
       <c r="AT2" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="AU2" s="13"/>
+      <c r="AU2" s="12"/>
       <c r="AV2" s="3" t="s">
         <v>55</v>
       </c>
@@ -1492,17 +1495,17 @@
       <c r="AX2" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="AY2" s="13"/>
+      <c r="AY2" s="12"/>
       <c r="AZ2" s="3" t="s">
         <v>58</v>
       </c>
       <c r="BA2" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="BB2" s="13"/>
-      <c r="BC2" s="13"/>
-    </row>
-    <row r="3" spans="1:55">
+      <c r="BB2" s="12"/>
+      <c r="BC2" s="12"/>
+    </row>
+    <row r="3" spans="1:56">
       <c r="A3">
         <v>1000</v>
       </c>
@@ -1574,31 +1577,32 @@
       <c r="AG3" s="4"/>
       <c r="AH3" s="4"/>
       <c r="AI3" s="4"/>
-      <c r="AJ3" s="4"/>
+      <c r="AJ3" s="4">
+        <v>232</v>
+      </c>
       <c r="AK3" s="4"/>
-      <c r="AL3" s="4">
-        <v>45782</v>
-      </c>
-      <c r="AM3" s="8"/>
+      <c r="AL3" s="4"/>
+      <c r="AM3" s="4"/>
       <c r="AN3" s="8"/>
-      <c r="AO3" s="7"/>
+      <c r="AO3" s="8"/>
       <c r="AP3" s="7"/>
-      <c r="AQ3" s="9"/>
-      <c r="AR3" s="7"/>
+      <c r="AQ3" s="7"/>
+      <c r="AR3" s="9"/>
       <c r="AS3" s="7"/>
-      <c r="AT3" s="4"/>
+      <c r="AT3" s="7"/>
       <c r="AU3" s="4"/>
-      <c r="AV3" s="8"/>
-      <c r="AW3" s="10">
+      <c r="AV3" s="4"/>
+      <c r="AW3" s="8"/>
+      <c r="AX3" s="10">
         <v>52.23</v>
       </c>
-      <c r="AX3" s="4"/>
-      <c r="AY3" s="7"/>
-      <c r="AZ3" s="9"/>
-      <c r="BA3" s="7"/>
+      <c r="AY3" s="4"/>
+      <c r="AZ3" s="7"/>
+      <c r="BA3" s="9"/>
       <c r="BB3" s="7"/>
-    </row>
-    <row r="4" spans="1:55">
+      <c r="BC3" s="7"/>
+    </row>
+    <row r="4" spans="1:56">
       <c r="A4">
         <v>1001</v>
       </c>
@@ -1666,24 +1670,25 @@
       <c r="AJ4" s="4"/>
       <c r="AK4" s="4"/>
       <c r="AL4" s="4"/>
-      <c r="AM4" s="8"/>
+      <c r="AM4" s="4"/>
       <c r="AN4" s="8"/>
-      <c r="AO4" s="7"/>
+      <c r="AO4" s="8"/>
       <c r="AP4" s="7"/>
-      <c r="AQ4" s="9"/>
-      <c r="AR4" s="7"/>
-      <c r="AS4" s="4"/>
+      <c r="AQ4" s="7"/>
+      <c r="AR4" s="9"/>
+      <c r="AS4" s="7"/>
       <c r="AT4" s="4"/>
       <c r="AU4" s="4"/>
-      <c r="AV4" s="8"/>
-      <c r="AW4" s="4"/>
+      <c r="AV4" s="4"/>
+      <c r="AW4" s="8"/>
       <c r="AX4" s="4"/>
-      <c r="AY4" s="7"/>
-      <c r="AZ4" s="9"/>
-      <c r="BA4" s="7"/>
+      <c r="AY4" s="4"/>
+      <c r="AZ4" s="7"/>
+      <c r="BA4" s="9"/>
       <c r="BB4" s="7"/>
-    </row>
-    <row r="5" spans="1:55">
+      <c r="BC4" s="7"/>
+    </row>
+    <row r="5" spans="1:56">
       <c r="A5">
         <v>1002</v>
       </c>
@@ -1756,26 +1761,27 @@
       <c r="AJ5" s="4"/>
       <c r="AK5" s="4"/>
       <c r="AL5" s="4"/>
-      <c r="AM5" s="8"/>
+      <c r="AM5" s="4"/>
       <c r="AN5" s="8"/>
-      <c r="AO5" s="7"/>
+      <c r="AO5" s="8"/>
       <c r="AP5" s="7"/>
-      <c r="AQ5" s="9"/>
-      <c r="AR5" s="7"/>
+      <c r="AQ5" s="7"/>
+      <c r="AR5" s="9"/>
       <c r="AS5" s="7"/>
-      <c r="AT5" s="4"/>
+      <c r="AT5" s="7"/>
       <c r="AU5" s="4"/>
-      <c r="AV5" s="8"/>
-      <c r="AW5" s="10">
+      <c r="AV5" s="4"/>
+      <c r="AW5" s="8"/>
+      <c r="AX5" s="10">
         <v>65.39</v>
       </c>
-      <c r="AX5" s="4"/>
-      <c r="AY5" s="7"/>
-      <c r="AZ5" s="9"/>
-      <c r="BA5" s="7"/>
+      <c r="AY5" s="4"/>
+      <c r="AZ5" s="7"/>
+      <c r="BA5" s="9"/>
       <c r="BB5" s="7"/>
-    </row>
-    <row r="6" spans="1:55">
+      <c r="BC5" s="7"/>
+    </row>
+    <row r="6" spans="1:56">
       <c r="A6">
         <v>1003</v>
       </c>
@@ -1843,24 +1849,25 @@
       <c r="AJ6" s="4"/>
       <c r="AK6" s="4"/>
       <c r="AL6" s="4"/>
-      <c r="AM6" s="8"/>
+      <c r="AM6" s="4"/>
       <c r="AN6" s="8"/>
-      <c r="AO6" s="4"/>
+      <c r="AO6" s="8"/>
       <c r="AP6" s="4"/>
-      <c r="AQ6" s="8"/>
-      <c r="AR6" s="4"/>
+      <c r="AQ6" s="4"/>
+      <c r="AR6" s="8"/>
       <c r="AS6" s="4"/>
       <c r="AT6" s="4"/>
       <c r="AU6" s="4"/>
-      <c r="AV6" s="8"/>
-      <c r="AW6" s="4"/>
+      <c r="AV6" s="4"/>
+      <c r="AW6" s="8"/>
       <c r="AX6" s="4"/>
       <c r="AY6" s="4"/>
-      <c r="AZ6" s="8"/>
-      <c r="BA6" s="4"/>
+      <c r="AZ6" s="4"/>
+      <c r="BA6" s="8"/>
       <c r="BB6" s="4"/>
-    </row>
-    <row r="7" spans="1:55">
+      <c r="BC6" s="4"/>
+    </row>
+    <row r="7" spans="1:56">
       <c r="A7">
         <v>1004</v>
       </c>
@@ -1930,24 +1937,25 @@
       <c r="AJ7" s="4"/>
       <c r="AK7" s="4"/>
       <c r="AL7" s="4"/>
-      <c r="AM7" s="8"/>
+      <c r="AM7" s="4"/>
       <c r="AN7" s="8"/>
-      <c r="AO7" s="7"/>
+      <c r="AO7" s="8"/>
       <c r="AP7" s="7"/>
-      <c r="AQ7" s="9"/>
-      <c r="AR7" s="7"/>
-      <c r="AS7" s="4"/>
+      <c r="AQ7" s="7"/>
+      <c r="AR7" s="9"/>
+      <c r="AS7" s="7"/>
       <c r="AT7" s="4"/>
       <c r="AU7" s="4"/>
-      <c r="AV7" s="8"/>
-      <c r="AW7" s="4"/>
+      <c r="AV7" s="4"/>
+      <c r="AW7" s="8"/>
       <c r="AX7" s="4"/>
-      <c r="AY7" s="7"/>
-      <c r="AZ7" s="9"/>
-      <c r="BA7" s="4"/>
-      <c r="BB7" s="7"/>
-    </row>
-    <row r="8" spans="1:55">
+      <c r="AY7" s="4"/>
+      <c r="AZ7" s="7"/>
+      <c r="BA7" s="9"/>
+      <c r="BB7" s="4"/>
+      <c r="BC7" s="7"/>
+    </row>
+    <row r="8" spans="1:56">
       <c r="A8">
         <v>1005</v>
       </c>
@@ -2023,28 +2031,29 @@
       <c r="AJ8" s="4"/>
       <c r="AK8" s="4"/>
       <c r="AL8" s="4"/>
-      <c r="AM8" s="8"/>
+      <c r="AM8" s="4"/>
       <c r="AN8" s="8"/>
-      <c r="AO8" s="7"/>
+      <c r="AO8" s="8"/>
       <c r="AP8" s="7"/>
-      <c r="AQ8" s="9"/>
-      <c r="AR8" s="7"/>
+      <c r="AQ8" s="7"/>
+      <c r="AR8" s="9"/>
       <c r="AS8" s="7"/>
-      <c r="AT8" s="4"/>
+      <c r="AT8" s="7"/>
       <c r="AU8" s="4"/>
-      <c r="AV8" s="6">
+      <c r="AV8" s="4"/>
+      <c r="AW8" s="6">
         <v>354.73</v>
       </c>
-      <c r="AW8" s="10">
+      <c r="AX8" s="10">
         <v>40.67</v>
       </c>
-      <c r="AX8" s="4"/>
-      <c r="AY8" s="7"/>
-      <c r="AZ8" s="9"/>
-      <c r="BA8" s="7"/>
+      <c r="AY8" s="4"/>
+      <c r="AZ8" s="7"/>
+      <c r="BA8" s="9"/>
       <c r="BB8" s="7"/>
-    </row>
-    <row r="9" spans="1:55">
+      <c r="BC8" s="7"/>
+    </row>
+    <row r="9" spans="1:56">
       <c r="A9">
         <v>1006</v>
       </c>
@@ -2106,24 +2115,25 @@
       <c r="AJ9" s="4"/>
       <c r="AK9" s="4"/>
       <c r="AL9" s="4"/>
-      <c r="AM9" s="8"/>
+      <c r="AM9" s="4"/>
       <c r="AN9" s="8"/>
-      <c r="AO9" s="7"/>
+      <c r="AO9" s="8"/>
       <c r="AP9" s="7"/>
-      <c r="AQ9" s="9"/>
-      <c r="AR9" s="7"/>
+      <c r="AQ9" s="7"/>
+      <c r="AR9" s="9"/>
       <c r="AS9" s="7"/>
-      <c r="AT9" s="4"/>
+      <c r="AT9" s="7"/>
       <c r="AU9" s="4"/>
-      <c r="AV9" s="8"/>
-      <c r="AW9" s="4"/>
+      <c r="AV9" s="4"/>
+      <c r="AW9" s="8"/>
       <c r="AX9" s="4"/>
-      <c r="AY9" s="7"/>
-      <c r="AZ9" s="9"/>
-      <c r="BA9" s="7"/>
+      <c r="AY9" s="4"/>
+      <c r="AZ9" s="7"/>
+      <c r="BA9" s="9"/>
       <c r="BB9" s="7"/>
-    </row>
-    <row r="10" spans="1:55">
+      <c r="BC9" s="7"/>
+    </row>
+    <row r="10" spans="1:56">
       <c r="A10">
         <v>1007</v>
       </c>
@@ -2197,24 +2207,25 @@
       <c r="AJ10" s="4"/>
       <c r="AK10" s="4"/>
       <c r="AL10" s="4"/>
-      <c r="AM10" s="8"/>
+      <c r="AM10" s="4"/>
       <c r="AN10" s="8"/>
-      <c r="AO10" s="7"/>
+      <c r="AO10" s="8"/>
       <c r="AP10" s="7"/>
-      <c r="AQ10" s="9"/>
-      <c r="AR10" s="7"/>
+      <c r="AQ10" s="7"/>
+      <c r="AR10" s="9"/>
       <c r="AS10" s="7"/>
-      <c r="AT10" s="4"/>
+      <c r="AT10" s="7"/>
       <c r="AU10" s="4"/>
-      <c r="AV10" s="8"/>
-      <c r="AW10" s="4"/>
+      <c r="AV10" s="4"/>
+      <c r="AW10" s="8"/>
       <c r="AX10" s="4"/>
-      <c r="AY10" s="7"/>
-      <c r="AZ10" s="9"/>
-      <c r="BA10" s="7"/>
+      <c r="AY10" s="4"/>
+      <c r="AZ10" s="7"/>
+      <c r="BA10" s="9"/>
       <c r="BB10" s="7"/>
-    </row>
-    <row r="11" spans="1:55">
+      <c r="BC10" s="7"/>
+    </row>
+    <row r="11" spans="1:56">
       <c r="A11">
         <v>1008</v>
       </c>
@@ -2279,24 +2290,25 @@
       <c r="AJ11" s="4"/>
       <c r="AK11" s="4"/>
       <c r="AL11" s="4"/>
-      <c r="AM11" s="8"/>
+      <c r="AM11" s="4"/>
       <c r="AN11" s="8"/>
-      <c r="AO11" s="7"/>
+      <c r="AO11" s="8"/>
       <c r="AP11" s="7"/>
-      <c r="AQ11" s="9"/>
-      <c r="AR11" s="7"/>
+      <c r="AQ11" s="7"/>
+      <c r="AR11" s="9"/>
       <c r="AS11" s="7"/>
-      <c r="AT11" s="4"/>
+      <c r="AT11" s="7"/>
       <c r="AU11" s="4"/>
-      <c r="AV11" s="8"/>
-      <c r="AW11" s="4"/>
+      <c r="AV11" s="4"/>
+      <c r="AW11" s="8"/>
       <c r="AX11" s="4"/>
-      <c r="AY11" s="7"/>
-      <c r="AZ11" s="9"/>
-      <c r="BA11" s="7"/>
+      <c r="AY11" s="4"/>
+      <c r="AZ11" s="7"/>
+      <c r="BA11" s="9"/>
       <c r="BB11" s="7"/>
-    </row>
-    <row r="12" spans="1:55">
+      <c r="BC11" s="7"/>
+    </row>
+    <row r="12" spans="1:56">
       <c r="A12">
         <v>1009</v>
       </c>
@@ -2367,24 +2379,25 @@
       <c r="AJ12" s="4"/>
       <c r="AK12" s="4"/>
       <c r="AL12" s="4"/>
-      <c r="AM12" s="8"/>
+      <c r="AM12" s="4"/>
       <c r="AN12" s="8"/>
-      <c r="AO12" s="7"/>
+      <c r="AO12" s="8"/>
       <c r="AP12" s="7"/>
-      <c r="AQ12" s="9"/>
-      <c r="AR12" s="7"/>
+      <c r="AQ12" s="7"/>
+      <c r="AR12" s="9"/>
       <c r="AS12" s="7"/>
       <c r="AT12" s="7"/>
-      <c r="AU12" s="4"/>
-      <c r="AV12" s="8"/>
-      <c r="AW12" s="4"/>
+      <c r="AU12" s="7"/>
+      <c r="AV12" s="4"/>
+      <c r="AW12" s="8"/>
       <c r="AX12" s="4"/>
-      <c r="AY12" s="7"/>
-      <c r="AZ12" s="9"/>
-      <c r="BA12" s="7"/>
+      <c r="AY12" s="4"/>
+      <c r="AZ12" s="7"/>
+      <c r="BA12" s="9"/>
       <c r="BB12" s="7"/>
-    </row>
-    <row r="13" spans="1:55">
+      <c r="BC12" s="7"/>
+    </row>
+    <row r="13" spans="1:56">
       <c r="A13">
         <v>1010</v>
       </c>
@@ -2459,27 +2472,28 @@
       <c r="AI13" s="7">
         <v>5563</v>
       </c>
-      <c r="AJ13" s="4"/>
+      <c r="AJ13" s="7"/>
       <c r="AK13" s="4"/>
       <c r="AL13" s="4"/>
-      <c r="AM13" s="9"/>
-      <c r="AN13" s="8"/>
-      <c r="AO13" s="7"/>
+      <c r="AM13" s="4"/>
+      <c r="AN13" s="9"/>
+      <c r="AO13" s="8"/>
       <c r="AP13" s="7"/>
-      <c r="AQ13" s="9"/>
-      <c r="AR13" s="7"/>
+      <c r="AQ13" s="7"/>
+      <c r="AR13" s="9"/>
       <c r="AS13" s="7"/>
-      <c r="AT13" s="4"/>
+      <c r="AT13" s="7"/>
       <c r="AU13" s="4"/>
-      <c r="AV13" s="8"/>
-      <c r="AW13" s="4"/>
+      <c r="AV13" s="4"/>
+      <c r="AW13" s="8"/>
       <c r="AX13" s="4"/>
-      <c r="AY13" s="7"/>
-      <c r="AZ13" s="9"/>
-      <c r="BA13" s="7"/>
+      <c r="AY13" s="4"/>
+      <c r="AZ13" s="7"/>
+      <c r="BA13" s="9"/>
       <c r="BB13" s="7"/>
-    </row>
-    <row r="14" spans="1:55">
+      <c r="BC13" s="7"/>
+    </row>
+    <row r="14" spans="1:56">
       <c r="A14">
         <v>1011</v>
       </c>
@@ -2544,24 +2558,25 @@
       <c r="AJ14" s="4"/>
       <c r="AK14" s="4"/>
       <c r="AL14" s="4"/>
-      <c r="AM14" s="8"/>
+      <c r="AM14" s="4"/>
       <c r="AN14" s="8"/>
-      <c r="AO14" s="7"/>
+      <c r="AO14" s="8"/>
       <c r="AP14" s="7"/>
-      <c r="AQ14" s="9"/>
-      <c r="AR14" s="7"/>
+      <c r="AQ14" s="7"/>
+      <c r="AR14" s="9"/>
       <c r="AS14" s="7"/>
-      <c r="AT14" s="4"/>
+      <c r="AT14" s="7"/>
       <c r="AU14" s="4"/>
-      <c r="AV14" s="8"/>
-      <c r="AW14" s="4"/>
+      <c r="AV14" s="4"/>
+      <c r="AW14" s="8"/>
       <c r="AX14" s="4"/>
-      <c r="AY14" s="7"/>
-      <c r="AZ14" s="9"/>
-      <c r="BA14" s="7"/>
+      <c r="AY14" s="4"/>
+      <c r="AZ14" s="7"/>
+      <c r="BA14" s="9"/>
       <c r="BB14" s="7"/>
-    </row>
-    <row r="15" spans="1:55">
+      <c r="BC14" s="7"/>
+    </row>
+    <row r="15" spans="1:56">
       <c r="A15">
         <v>1012</v>
       </c>
@@ -2634,26 +2649,27 @@
       <c r="AJ15" s="4"/>
       <c r="AK15" s="4"/>
       <c r="AL15" s="4"/>
-      <c r="AM15" s="8"/>
+      <c r="AM15" s="4"/>
       <c r="AN15" s="8"/>
-      <c r="AO15" s="7"/>
+      <c r="AO15" s="8"/>
       <c r="AP15" s="7"/>
-      <c r="AQ15" s="9"/>
-      <c r="AR15" s="7"/>
+      <c r="AQ15" s="7"/>
+      <c r="AR15" s="9"/>
       <c r="AS15" s="7"/>
-      <c r="AT15" s="4"/>
+      <c r="AT15" s="7"/>
       <c r="AU15" s="4"/>
-      <c r="AV15" s="8"/>
-      <c r="AW15" s="10">
+      <c r="AV15" s="4"/>
+      <c r="AW15" s="8"/>
+      <c r="AX15" s="10">
         <v>35.75</v>
       </c>
-      <c r="AX15" s="4"/>
-      <c r="AY15" s="7"/>
-      <c r="AZ15" s="9"/>
-      <c r="BA15" s="7"/>
+      <c r="AY15" s="4"/>
+      <c r="AZ15" s="7"/>
+      <c r="BA15" s="9"/>
       <c r="BB15" s="7"/>
-    </row>
-    <row r="16" spans="1:55">
+      <c r="BC15" s="7"/>
+    </row>
+    <row r="16" spans="1:56">
       <c r="A16">
         <v>1013</v>
       </c>
@@ -2728,27 +2744,27 @@
       <c r="AI16" s="7">
         <v>5547.5</v>
       </c>
-      <c r="AJ16" s="4"/>
+      <c r="AJ16" s="7"/>
       <c r="AK16" s="4"/>
       <c r="AL16" s="4"/>
-      <c r="AM16" s="8"/>
       <c r="AN16" s="8"/>
-      <c r="AO16" s="7"/>
+      <c r="AO16" s="8"/>
       <c r="AP16" s="7"/>
-      <c r="AQ16" s="9"/>
-      <c r="AR16" s="7"/>
+      <c r="AQ16" s="7"/>
+      <c r="AR16" s="9"/>
       <c r="AS16" s="7"/>
-      <c r="AT16" s="4"/>
+      <c r="AT16" s="7"/>
       <c r="AU16" s="4"/>
-      <c r="AV16" s="8"/>
-      <c r="AW16" s="4"/>
+      <c r="AV16" s="4"/>
+      <c r="AW16" s="8"/>
       <c r="AX16" s="4"/>
-      <c r="AY16" s="7"/>
-      <c r="AZ16" s="9"/>
-      <c r="BA16" s="7"/>
+      <c r="AY16" s="4"/>
+      <c r="AZ16" s="7"/>
+      <c r="BA16" s="9"/>
       <c r="BB16" s="7"/>
-    </row>
-    <row r="17" spans="1:49">
+      <c r="BC16" s="7"/>
+    </row>
+    <row r="17" spans="1:50">
       <c r="A17">
         <v>1014</v>
       </c>
@@ -2805,7 +2821,7 @@
         <v>4507.87</v>
       </c>
     </row>
-    <row r="18" spans="1:49">
+    <row r="18" spans="1:50">
       <c r="A18">
         <v>1015</v>
       </c>
@@ -2858,7 +2874,7 @@
         <v>2867</v>
       </c>
     </row>
-    <row r="19" spans="1:49">
+    <row r="19" spans="1:50">
       <c r="A19">
         <v>1016</v>
       </c>
@@ -2911,7 +2927,7 @@
         <v>3277.67</v>
       </c>
     </row>
-    <row r="20" spans="1:49">
+    <row r="20" spans="1:50">
       <c r="A20">
         <v>1017</v>
       </c>
@@ -2964,7 +2980,7 @@
         <v>2525.5</v>
       </c>
     </row>
-    <row r="21" spans="1:49">
+    <row r="21" spans="1:50">
       <c r="A21">
         <v>1018</v>
       </c>
@@ -3020,7 +3036,7 @@
         <v>6166.67</v>
       </c>
     </row>
-    <row r="22" spans="1:49">
+    <row r="22" spans="1:50">
       <c r="A22">
         <v>1019</v>
       </c>
@@ -3079,7 +3095,7 @@
         <v>52.23</v>
       </c>
     </row>
-    <row r="23" spans="1:49">
+    <row r="23" spans="1:50">
       <c r="A23">
         <v>1020</v>
       </c>
@@ -3133,7 +3149,7 @@
       </c>
       <c r="AA23" s="4"/>
     </row>
-    <row r="24" spans="1:49">
+    <row r="24" spans="1:50">
       <c r="A24">
         <v>1021</v>
       </c>
@@ -3192,7 +3208,7 @@
         <v>65.39</v>
       </c>
     </row>
-    <row r="25" spans="1:49">
+    <row r="25" spans="1:50">
       <c r="A25">
         <v>1022</v>
       </c>
@@ -3243,7 +3259,7 @@
       </c>
       <c r="AA25" s="4"/>
     </row>
-    <row r="26" spans="1:49">
+    <row r="26" spans="1:50">
       <c r="A26">
         <v>1023</v>
       </c>
@@ -3296,11 +3312,11 @@
         <v>0</v>
       </c>
       <c r="AA26" s="4"/>
-      <c r="AW26">
+      <c r="AX26">
         <v>55.7</v>
       </c>
     </row>
-    <row r="27" spans="1:49">
+    <row r="27" spans="1:50">
       <c r="A27">
         <v>1024</v>
       </c>
@@ -3359,7 +3375,7 @@
         <v>40.67</v>
       </c>
     </row>
-    <row r="28" spans="1:49">
+    <row r="28" spans="1:50">
       <c r="A28">
         <v>1025</v>
       </c>
@@ -3413,7 +3429,7 @@
       </c>
       <c r="AA28" s="4"/>
     </row>
-    <row r="29" spans="1:49">
+    <row r="29" spans="1:50">
       <c r="A29">
         <v>1026</v>
       </c>
@@ -3470,7 +3486,7 @@
       </c>
       <c r="AA29" s="4"/>
     </row>
-    <row r="30" spans="1:49">
+    <row r="30" spans="1:50">
       <c r="A30">
         <v>1027</v>
       </c>
@@ -3527,7 +3543,7 @@
       </c>
       <c r="AA30" s="4"/>
     </row>
-    <row r="31" spans="1:49">
+    <row r="31" spans="1:50">
       <c r="A31">
         <v>1028</v>
       </c>
@@ -3583,11 +3599,11 @@
         <v>2666.67</v>
       </c>
       <c r="AA31" s="4"/>
-      <c r="AW31">
+      <c r="AX31">
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:49">
+    <row r="32" spans="1:50">
       <c r="A32">
         <v>1029</v>
       </c>
@@ -3641,7 +3657,7 @@
       </c>
       <c r="AA32" s="4"/>
     </row>
-    <row r="33" spans="1:54">
+    <row r="33" spans="1:55">
       <c r="A33">
         <v>1030</v>
       </c>
@@ -3694,11 +3710,11 @@
         <v>4507.87</v>
       </c>
       <c r="AA33" s="4"/>
-      <c r="AW33">
+      <c r="AX33">
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:54">
+    <row r="34" spans="1:55">
       <c r="A34">
         <v>1031</v>
       </c>
@@ -3754,7 +3770,7 @@
         <v>35.75</v>
       </c>
     </row>
-    <row r="35" spans="1:54">
+    <row r="35" spans="1:55">
       <c r="A35">
         <v>1032</v>
       </c>
@@ -3809,11 +3825,11 @@
       <c r="Z35">
         <v>3550</v>
       </c>
-      <c r="AW35">
+      <c r="AX35">
         <v>0.76</v>
       </c>
     </row>
-    <row r="36" spans="1:54">
+    <row r="36" spans="1:55">
       <c r="A36">
         <v>1033</v>
       </c>
@@ -3869,7 +3885,7 @@
         <v>2098.5</v>
       </c>
     </row>
-    <row r="37" spans="1:54">
+    <row r="37" spans="1:55">
       <c r="A37">
         <v>1034</v>
       </c>
@@ -3922,7 +3938,7 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="38" spans="1:54">
+    <row r="38" spans="1:55">
       <c r="A38">
         <v>1035</v>
       </c>
@@ -3977,8 +3993,9 @@
       <c r="Z38" s="6">
         <v>2250</v>
       </c>
-    </row>
-    <row r="39" spans="1:54">
+      <c r="AM38" s="4"/>
+    </row>
+    <row r="39" spans="1:55">
       <c r="Y39" t="s">
         <v>251</v>
       </c>
@@ -4012,29 +4029,26 @@
       <c r="AI39" s="4">
         <v>11110.5</v>
       </c>
-      <c r="AJ39" s="4">
-        <v>0</v>
-      </c>
+      <c r="AJ39" s="4"/>
       <c r="AK39" s="4">
         <v>0</v>
       </c>
-      <c r="AL39" s="4"/>
-      <c r="AM39" s="8">
+      <c r="AL39" s="4">
         <v>0</v>
       </c>
       <c r="AN39" s="8">
         <v>0</v>
       </c>
-      <c r="AO39" s="4">
+      <c r="AO39" s="8">
         <v>0</v>
       </c>
       <c r="AP39" s="4">
         <v>0</v>
       </c>
-      <c r="AQ39" s="8">
+      <c r="AQ39" s="4">
         <v>0</v>
       </c>
-      <c r="AR39" s="4">
+      <c r="AR39" s="8">
         <v>0</v>
       </c>
       <c r="AS39" s="4">
@@ -4046,65 +4060,62 @@
       <c r="AU39" s="4">
         <v>0</v>
       </c>
-      <c r="AV39" s="8">
+      <c r="AV39" s="4">
+        <v>0</v>
+      </c>
+      <c r="AW39" s="8">
         <v>354.73</v>
       </c>
-      <c r="AW39" s="4">
+      <c r="AX39" s="4">
         <v>194.04</v>
-      </c>
-      <c r="AX39" s="4">
-        <v>0</v>
       </c>
       <c r="AY39" s="4">
         <v>0</v>
       </c>
-      <c r="AZ39" s="8">
+      <c r="AZ39" s="4">
         <v>0</v>
       </c>
-      <c r="BA39" s="4">
+      <c r="BA39" s="8">
         <v>0</v>
       </c>
       <c r="BB39" s="4">
         <v>0</v>
       </c>
+      <c r="BC39" s="4">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="35">
+  <mergeCells count="29">
+    <mergeCell ref="AW1:AY1"/>
+    <mergeCell ref="BA1:BB1"/>
+    <mergeCell ref="Z1:AL1"/>
+    <mergeCell ref="AR1:AU1"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="W1:W2"/>
+    <mergeCell ref="X1:X2"/>
+    <mergeCell ref="Y1:Y2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="V1:V2"/>
-    <mergeCell ref="W1:W2"/>
-    <mergeCell ref="X1:X2"/>
-    <mergeCell ref="Y1:Y2"/>
-    <mergeCell ref="Z1:AK1"/>
-    <mergeCell ref="AO1:AO2"/>
-    <mergeCell ref="AP1:AP2"/>
-    <mergeCell ref="AQ1:AT1"/>
-    <mergeCell ref="AU1:AU2"/>
-    <mergeCell ref="AV1:AX1"/>
-    <mergeCell ref="AY1:AY2"/>
-    <mergeCell ref="AZ1:BA1"/>
-    <mergeCell ref="BB1:BB2"/>
-    <mergeCell ref="BC1:BC2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>